<commit_message>
updated example spreadsheets and generated bundles to latest v3 spec updates
</commit_message>
<xml_diff>
--- a/example-input/10X_v2_pbmc8k.xlsx
+++ b/example-input/10X_v2_pbmc8k.xlsx
@@ -67,9 +67,6 @@
     <t>seq.paired_ends</t>
   </si>
   <si>
-    <t>single_cell.method</t>
-  </si>
-  <si>
     <t>seq.molecule</t>
   </si>
   <si>
@@ -85,9 +82,6 @@
     <t>seq.machine</t>
   </si>
   <si>
-    <t>reads</t>
-  </si>
-  <si>
     <t>format</t>
   </si>
   <si>
@@ -133,15 +127,6 @@
     <t>index</t>
   </si>
   <si>
-    <t>single_cell.cell_barcode_offset</t>
-  </si>
-  <si>
-    <t>single_cell.cell_barcode_size</t>
-  </si>
-  <si>
-    <t>single_cell.cell_barcode_read</t>
-  </si>
-  <si>
     <t>pbmc8k_S1_L008_R1_001.fastq.gz</t>
   </si>
   <si>
@@ -196,18 +181,6 @@
     <t>rna.library_construction</t>
   </si>
   <si>
-    <t>10xV2</t>
-  </si>
-  <si>
-    <t>seq.umi_barcode_offset</t>
-  </si>
-  <si>
-    <t>seq.umi_barcode_read</t>
-  </si>
-  <si>
-    <t>seq.umi_barcode_size</t>
-  </si>
-  <si>
     <t>seq.lanes</t>
   </si>
   <si>
@@ -254,6 +227,33 @@
   </si>
   <si>
     <t>10X Genomics Inc.</t>
+  </si>
+  <si>
+    <t>r1</t>
+  </si>
+  <si>
+    <t>r2</t>
+  </si>
+  <si>
+    <t>single_cell.cell_handling</t>
+  </si>
+  <si>
+    <t>single_cell.barcode.offset</t>
+  </si>
+  <si>
+    <t>single_cell.barcode.read</t>
+  </si>
+  <si>
+    <t>single_cell.barcode.size</t>
+  </si>
+  <si>
+    <t>seq.umi_barcode.offset</t>
+  </si>
+  <si>
+    <t>seq.umi_barcode.size</t>
+  </si>
+  <si>
+    <t>seq.umi_barcode.read</t>
   </si>
 </sst>
 </file>
@@ -309,8 +309,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -330,7 +342,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="27">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -338,6 +350,12 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -345,6 +363,12 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -657,15 +681,15 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -673,7 +697,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -693,10 +717,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="B1" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -704,47 +728,47 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B4" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="B6" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="B7" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -767,7 +791,7 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -797,16 +821,16 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F1" t="s">
         <v>0</v>
@@ -817,25 +841,25 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
         <v>21</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" t="s">
         <v>23</v>
-      </c>
-      <c r="E2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -870,18 +894,18 @@
         <v>5</v>
       </c>
       <c r="D1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="F1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B2">
         <v>9606</v>
@@ -893,7 +917,7 @@
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="F2">
         <v>9606</v>
@@ -922,8 +946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -937,7 +961,8 @@
     <col min="7" max="7" width="25" customWidth="1"/>
     <col min="8" max="8" width="31.83203125" customWidth="1"/>
     <col min="9" max="10" width="22.83203125" customWidth="1"/>
-    <col min="11" max="12" width="12.5" customWidth="1"/>
+    <col min="11" max="11" width="12.5" customWidth="1"/>
+    <col min="12" max="12" width="32" customWidth="1"/>
     <col min="13" max="13" width="24" customWidth="1"/>
     <col min="14" max="14" width="19.1640625" customWidth="1"/>
     <col min="15" max="16" width="24" customWidth="1"/>
@@ -950,49 +975,49 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>66</v>
       </c>
       <c r="C1" t="s">
-        <v>32</v>
+        <v>67</v>
       </c>
       <c r="D1" t="s">
-        <v>34</v>
+        <v>68</v>
       </c>
       <c r="E1" t="s">
-        <v>33</v>
+        <v>69</v>
       </c>
       <c r="F1" t="s">
         <v>9</v>
       </c>
       <c r="G1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H1" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="I1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K1" t="s">
         <v>13</v>
       </c>
-      <c r="J1" t="s">
-        <v>50</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M1" t="s">
         <v>14</v>
       </c>
-      <c r="L1" t="s">
-        <v>52</v>
-      </c>
-      <c r="M1" t="s">
-        <v>15</v>
-      </c>
       <c r="N1" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="O1" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="P1" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>8</v>
@@ -1000,55 +1025,55 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E2">
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H2">
         <v>16</v>
       </c>
       <c r="I2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="J2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="K2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L2" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="M2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="N2">
         <v>10</v>
       </c>
       <c r="O2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="P2" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
@@ -1065,7 +1090,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1079,13 +1104,13 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="C1" t="s">
-        <v>31</v>
+        <v>64</v>
       </c>
       <c r="D1" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -1096,10 +1121,10 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1110,10 +1135,10 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1139,39 +1164,39 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>